<commit_message>
add new config json
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="1">
   <si>
-    <t>5H98jLSSw9VYxuxMDZvkjf5Zdgc1BZQSnnk44ziyei12PvqP</t>
+    <t>5CYTXhvrfnK2Zmt49aEnGZoJWJk8TSQUC1sMT3tehitaoyuq</t>
   </si>
 </sst>
 </file>
@@ -57,7 +57,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -65,6 +65,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -303,7 +306,7 @@
       <c r="B2" s="2">
         <v>2.0</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>1000.0</v>
       </c>
     </row>
@@ -347,8 +350,8 @@
       <c r="B6" s="2">
         <v>6.0</v>
       </c>
-      <c r="C6" s="2">
-        <v>1000.0</v>
+      <c r="C6" s="3">
+        <v>2000.0</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
@@ -358,8 +361,8 @@
       <c r="B7" s="2">
         <v>7.0</v>
       </c>
-      <c r="C7" s="2">
-        <v>1000.0</v>
+      <c r="C7" s="3">
+        <v>2000.0</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
@@ -369,8 +372,8 @@
       <c r="B8" s="2">
         <v>8.0</v>
       </c>
-      <c r="C8" s="2">
-        <v>1000.0</v>
+      <c r="C8" s="3">
+        <v>2000.0</v>
       </c>
     </row>
     <row r="9" ht="14.25" customHeight="1">
@@ -380,8 +383,8 @@
       <c r="B9" s="2">
         <v>9.0</v>
       </c>
-      <c r="C9" s="2">
-        <v>1000.0</v>
+      <c r="C9" s="3">
+        <v>2000.0</v>
       </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
@@ -391,8 +394,8 @@
       <c r="B10" s="2">
         <v>10.0</v>
       </c>
-      <c r="C10" s="2">
-        <v>1000.0</v>
+      <c r="C10" s="3">
+        <v>2000.0</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1"/>

</xml_diff>